<commit_message>
Added new line of data.
</commit_message>
<xml_diff>
--- a/Incense.xlsx
+++ b/Incense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmand\Documents\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmand\Documents\GitHub\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D9EEB6-C640-42F7-8717-E5C71A48E55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2629FA4-7FEF-41F1-B322-463AC20E402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3690" windowWidth="24240" windowHeight="13140" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
+    <workbookView xWindow="1860" yWindow="2010" windowWidth="21960" windowHeight="14400" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Candy Apple</t>
+  </si>
+  <si>
+    <t>Goregasm</t>
+  </si>
+  <si>
+    <t>Nightshade</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8D868B-B829-4C59-819F-F583A548F3DE}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,6 +798,174 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45463</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45469</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45474</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45477</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45481</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45485</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45488</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45491</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45494</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45501</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45505</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45507</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added lines to dataset
</commit_message>
<xml_diff>
--- a/Incense.xlsx
+++ b/Incense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmand\Documents\GitHub\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2629FA4-7FEF-41F1-B322-463AC20E402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF936A0-1CB1-4FD7-A731-6A74C0FC9D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2010" windowWidth="21960" windowHeight="14400" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
+    <workbookView xWindow="14550" yWindow="4005" windowWidth="21960" windowHeight="14400" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8D868B-B829-4C59-819F-F583A548F3DE}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,6 +966,76 @@
         <v>1</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45517</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45523</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45524</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45525</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45526</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new data line
</commit_message>
<xml_diff>
--- a/Incense.xlsx
+++ b/Incense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmand\Documents\GitHub\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF936A0-1CB1-4FD7-A731-6A74C0FC9D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B849E9-B351-4E5A-BE27-EFBC6E33CB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14550" yWindow="4005" windowWidth="21960" windowHeight="14400" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
+    <workbookView xWindow="10035" yWindow="2505" windowWidth="27015" windowHeight="14895" xr2:uid="{732C5B80-8AC8-4CEC-9E59-4259BC7ED0EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -462,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8D868B-B829-4C59-819F-F583A548F3DE}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1036,6 +1036,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45580</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>